<commit_message>
a few more scripting ideas
</commit_message>
<xml_diff>
--- a/automate_excel/mhkendofyear/mhkendofyear.xlsx
+++ b/automate_excel/mhkendofyear/mhkendofyear.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CustomOfficeTemplates\current_code\MyScripts\automate_excel\mhkendofyear\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E83808C-7560-47AC-BBF2-8538307496D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC2410E-E0C4-4210-B896-430EEA55760E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1692" windowWidth="17280" windowHeight="8964" xr2:uid="{AE337C70-081B-4C59-88D3-A065B7267D1B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AE337C70-081B-4C59-88D3-A065B7267D1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="125">
   <si>
     <t>CLIENT</t>
   </si>
@@ -111,12 +111,6 @@
   </si>
   <si>
     <t>ELD</t>
-  </si>
-  <si>
-    <t>Lance H. (Lance is not shown as a contact in Scope for Elderplan)</t>
-  </si>
-  <si>
-    <t>35266 (scope not completed)</t>
   </si>
   <si>
     <t>EIC</t>
@@ -671,7 +665,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -730,6 +724,8 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
@@ -1047,9 +1043,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4094E6FF-A45D-4E89-ABB8-4156E5D7A144}">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A17" sqref="A17"/>
+      <selection pane="topRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1095,31 +1091,31 @@
         <v>6</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I1" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="L1" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="M1" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="N1" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="O1" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="P1" s="25" t="s">
         <v>66</v>
-      </c>
-      <c r="O1" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="P1" s="25" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -1135,28 +1131,28 @@
       <c r="G2" s="12"/>
       <c r="H2" s="13"/>
       <c r="I2" s="26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J2" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K2" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L2" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M2" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N2" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O2" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="P2" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -1172,28 +1168,28 @@
       <c r="G3" s="12"/>
       <c r="H3" s="13"/>
       <c r="I3" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L3" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M3" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N3" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O3" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="P3" s="26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -1216,28 +1212,28 @@
       </c>
       <c r="H4" s="13"/>
       <c r="I4" s="26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J4" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K4" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L4" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M4" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N4" s="26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O4" s="26" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="P4" s="26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -1260,28 +1256,28 @@
       </c>
       <c r="H5" s="13"/>
       <c r="I5" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J5" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K5" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L5" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M5" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N5" s="26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O5" s="26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="P5" s="26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -1294,28 +1290,28 @@
       <c r="G6" s="12"/>
       <c r="H6" s="13"/>
       <c r="I6" s="26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J6" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K6" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L6" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M6" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N6" s="26" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O6" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="P6" s="26" t="s">
         <v>109</v>
-      </c>
-      <c r="P6" s="26" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -1338,28 +1334,28 @@
       </c>
       <c r="H7" s="13"/>
       <c r="I7" s="26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J7" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K7" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L7" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M7" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N7" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O7" s="26" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="P7" s="26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -1375,28 +1371,28 @@
       <c r="G8" s="12"/>
       <c r="H8" s="13"/>
       <c r="I8" s="26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J8" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K8" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L8" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M8" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N8" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O8" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="P8" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -1419,28 +1415,28 @@
       </c>
       <c r="H9" s="13"/>
       <c r="I9" s="26" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L9" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M9" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N9" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O9" s="26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="P9" s="26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -1448,174 +1444,174 @@
         <v>25</v>
       </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>27</v>
+      <c r="C10" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="29">
+        <v>35266</v>
       </c>
       <c r="E10" s="11">
         <v>25</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="J10" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="K10" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="L10" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="M10" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="N10" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="O10" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="P10" s="26" t="s">
         <v>89</v>
-      </c>
-      <c r="J10" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="K10" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="L10" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="M10" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="N10" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="O10" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="P10" s="26" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="12"/>
       <c r="H11" s="13"/>
       <c r="I11" s="26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J11" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K11" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L11" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M11" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N11" s="26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O11" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="P11" s="26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E12" s="11">
         <v>35</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H12" s="13"/>
       <c r="I12" s="26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K12" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L12" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M12" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N12" s="26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O12" s="26" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="P12" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E13" s="11">
         <v>30</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H13" s="13"/>
       <c r="I13" s="26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J13" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K13" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L13" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M13" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N13" s="26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O13" s="26" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="P13" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="16" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D14" s="10">
         <v>35268</v>
@@ -1625,41 +1621,41 @@
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J14" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K14" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L14" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M14" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N14" s="26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O14" s="26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="P14" s="26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="31.8" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D15" s="10">
         <v>35271</v>
@@ -1669,41 +1665,41 @@
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J15" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K15" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L15" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M15" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N15" s="26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O15" s="26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="P15" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D16" s="10">
         <v>35272</v>
@@ -1713,37 +1709,37 @@
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H16" s="13"/>
       <c r="I16" s="26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J16" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K16" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L16" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M16" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N16" s="26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O16" s="26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="P16" s="26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="9" t="s">
@@ -1757,152 +1753,152 @@
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H17" s="13"/>
       <c r="I17" s="26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J17" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K17" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L17" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M17" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N17" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O17" s="26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="P17" s="26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="12"/>
       <c r="H18" s="13"/>
       <c r="I18" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="J18" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="K18" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="L18" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="M18" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="N18" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="O18" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="P18" s="26" t="s">
         <v>98</v>
-      </c>
-      <c r="J18" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="K18" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="L18" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="M18" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="N18" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="O18" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="P18" s="26" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="12"/>
       <c r="H19" s="13"/>
       <c r="I19" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="J19" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="K19" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="L19" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="M19" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="N19" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="O19" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="P19" s="26" t="s">
         <v>101</v>
-      </c>
-      <c r="J19" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="K19" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="L19" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="M19" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="N19" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="O19" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="P19" s="26" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="12"/>
       <c r="H20" s="13"/>
       <c r="I20" s="26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J20" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K20" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L20" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M20" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N20" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="O20" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="P20" s="26" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D21" s="10">
         <v>35274</v>
@@ -1910,41 +1906,41 @@
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H21" s="13"/>
       <c r="I21" s="26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J21" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K21" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L21" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M21" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N21" s="26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O21" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="P21" s="26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D22" s="10">
         <v>35276</v>
@@ -1954,43 +1950,43 @@
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I22" s="26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J22" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K22" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L22" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M22" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N22" s="26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O22" s="26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="P22" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D23" s="10">
         <v>35277</v>
@@ -2000,43 +1996,43 @@
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I23" s="26" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J23" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K23" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L23" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M23" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N23" s="26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O23" s="26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="P23" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D24" s="10">
         <v>35278</v>
@@ -2046,37 +2042,37 @@
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H24" s="13"/>
       <c r="I24" s="26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J24" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K24" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L24" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M24" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N24" s="26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O24" s="26" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="P24" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="9" t="s">
@@ -2090,78 +2086,78 @@
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H25" s="13"/>
       <c r="I25" s="26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J25" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K25" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L25" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M25" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N25" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O25" s="26" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="P25" s="26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E26" s="11">
         <v>40</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H26" s="13"/>
       <c r="I26" s="26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J26" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K26" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L26" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M26" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N26" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="O26" s="26" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="P26" s="26" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="9" t="s">
@@ -2175,32 +2171,32 @@
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H27" s="13"/>
       <c r="I27" s="26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J27" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K27" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L27" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M27" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N27" s="26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O27" s="26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="P27" s="26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>